<commit_message>
Se añade las tuercas M3 a la fuente d ela P6.67
</commit_message>
<xml_diff>
--- a/P6,67/Escandallo Aveiro P6.76.xlsx
+++ b/P6,67/Escandallo Aveiro P6.76.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INGENIERIA ImasD\Desktop\Proyectos\Cruz AVEIRO\P6,67\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ingenieria ImasD\Desktop\Proyectos\Cruz-AVEIRO\P6,67\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2E9269-9B31-46B8-9B65-58ACDC0769C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4634DA-00A8-4A46-ABB3-C0848E40B57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$101</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>CRUZ</t>
   </si>
@@ -159,10 +159,13 @@
     <t>Receiving Card Placa expansora modelo A5s PLUS</t>
   </si>
   <si>
-    <t>Cable plano 20 vías 80 cm H-H</t>
-  </si>
-  <si>
-    <t>Cable plano 20 vías 20 cm H-H</t>
+    <t>Cable plano 20 vías 40 cm H-H</t>
+  </si>
+  <si>
+    <t>Cable plano 20 vías 90 cm H-H</t>
+  </si>
+  <si>
+    <t>Torreta L=30 H-M</t>
   </si>
 </sst>
 </file>
@@ -335,8 +338,8 @@
       <xdr:rowOff>7920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>199887</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
@@ -353,8 +356,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2982960" y="166670"/>
-          <a:ext cx="5487940" cy="442780"/>
+          <a:off x="2982960" y="169845"/>
+          <a:ext cx="5760990" cy="449130"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -574,13 +577,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>31751</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7155559</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
       <xdr:row>101</xdr:row>
       <xdr:rowOff>24305</xdr:rowOff>
     </xdr:to>
@@ -605,8 +608,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="31750" y="7308850"/>
-          <a:ext cx="7123809" cy="8761905"/>
+          <a:off x="31751" y="7634968"/>
+          <a:ext cx="7901213" cy="8881194"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -918,20 +921,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A6:E44"/>
+  <dimension ref="A6:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="106.90625" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" customWidth="1"/>
+    <col min="1" max="1" width="106.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -953,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -967,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -981,9 +984,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3">
         <v>4</v>
@@ -995,9 +998,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3">
         <v>6</v>
@@ -1009,7 +1012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1061,7 +1064,7 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1093,12 +1096,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>20</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>24</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>27</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>29</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>31</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>32</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>33</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>35</v>
       </c>
@@ -1266,7 +1269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>36</v>
       </c>
@@ -1274,9 +1277,25 @@
         <v>4</v>
       </c>
     </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="63" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="58" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>